<commit_message>
Implementation en cours de l'ecran.
</commit_message>
<xml_diff>
--- a/Ecrans.xlsx
+++ b/Ecrans.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Ext :</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Recyclage / Arret</t>
+  </si>
+  <si>
+    <t>EXT</t>
   </si>
 </sst>
 </file>
@@ -320,34 +323,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -650,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:I8"/>
+  <dimension ref="B1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5703125" defaultRowHeight="15"/>
@@ -663,32 +666,32 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:9" ht="15" customHeight="1">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="17"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="19"/>
     </row>
     <row r="3" spans="2:9" ht="15.75">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="13"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="2" t="s">
@@ -760,6 +763,11 @@
       <c r="G8" s="7"/>
       <c r="I8" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9">
+      <c r="I18" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>